<commit_message>
UI and Form Builder Update
</commit_message>
<xml_diff>
--- a/TrackModel/src/database.xlsx
+++ b/TrackModel/src/database.xlsx
@@ -369,13 +369,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,8 +403,17 @@
       <c r="I1">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1">
+        <v>0</v>
+      </c>
+      <c r="K1">
+        <v>0</v>
+      </c>
+      <c r="L1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -432,8 +441,17 @@
       <c r="I2">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -461,8 +479,17 @@
       <c r="I3">
         <v>72</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -490,8 +517,17 @@
       <c r="I4">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -519,8 +555,17 @@
       <c r="I5">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -540,7 +585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -568,8 +613,17 @@
       <c r="I7">
         <v>72</v>
       </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -597,8 +651,17 @@
       <c r="I8">
         <v>72</v>
       </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -626,8 +689,17 @@
       <c r="I9">
         <v>72</v>
       </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -655,8 +727,17 @@
       <c r="I10">
         <v>72</v>
       </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -684,8 +765,17 @@
       <c r="I11">
         <v>72</v>
       </c>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -699,7 +789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -727,8 +817,17 @@
       <c r="I13">
         <v>72</v>
       </c>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -756,8 +855,17 @@
       <c r="I14">
         <v>72</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -785,8 +893,17 @@
       <c r="I15">
         <v>72</v>
       </c>
-    </row>
-    <row r="16" spans="1:9">
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -814,8 +931,17 @@
       <c r="I16">
         <v>72</v>
       </c>
-    </row>
-    <row r="17" spans="1:9">
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -843,8 +969,17 @@
       <c r="I17">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="1:9">
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Not working Connection Service
</commit_message>
<xml_diff>
--- a/TrackModel/src/database.xlsx
+++ b/TrackModel/src/database.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L172"/>
+  <dimension ref="A1:M172"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,7 +452,7 @@
         <v>0</v>
       </c>
       <c r="I1" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J1" t="n">
         <v>0</v>
@@ -461,6 +461,9 @@
         <v>0</v>
       </c>
       <c r="L1" t="n">
+        <v>0</v>
+      </c>
+      <c r="M1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -496,7 +499,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -506,6 +509,9 @@
       </c>
       <c r="L2" t="n">
         <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -563,7 +569,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J4" t="n">
         <v>0</v>
@@ -573,6 +579,9 @@
       </c>
       <c r="L4" t="n">
         <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="5">
@@ -607,7 +616,7 @@
         <v>2</v>
       </c>
       <c r="I5" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
@@ -617,6 +626,9 @@
       </c>
       <c r="L5" t="n">
         <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -651,7 +663,7 @@
         <v>3</v>
       </c>
       <c r="I6" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
         <v>0</v>
@@ -661,6 +673,9 @@
       </c>
       <c r="L6" t="n">
         <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>8</v>
       </c>
     </row>
     <row r="7">
@@ -695,7 +710,7 @@
         <v>4</v>
       </c>
       <c r="I7" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J7" t="n">
         <v>0</v>
@@ -705,6 +720,9 @@
       </c>
       <c r="L7" t="n">
         <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -739,7 +757,7 @@
         <v>5</v>
       </c>
       <c r="I8" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -749,6 +767,9 @@
       </c>
       <c r="L8" t="n">
         <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="9">
@@ -783,7 +804,7 @@
         <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J9" t="n">
         <v>0</v>
@@ -793,6 +814,9 @@
       </c>
       <c r="L9" t="n">
         <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>17</v>
       </c>
     </row>
     <row r="10">
@@ -827,7 +851,7 @@
         <v>-5</v>
       </c>
       <c r="I10" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J10" t="n">
         <v>0</v>
@@ -837,6 +861,9 @@
       </c>
       <c r="L10" t="n">
         <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>12</v>
       </c>
     </row>
     <row r="11">
@@ -894,7 +921,7 @@
         <v>-4</v>
       </c>
       <c r="I12" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
         <v>0</v>
@@ -904,6 +931,9 @@
       </c>
       <c r="L12" t="n">
         <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="13">
@@ -938,7 +968,7 @@
         <v>-4</v>
       </c>
       <c r="I13" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
         <v>0</v>
@@ -948,6 +978,9 @@
       </c>
       <c r="L13" t="n">
         <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="14">
@@ -982,7 +1015,7 @@
         <v>-3</v>
       </c>
       <c r="I14" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J14" t="n">
         <v>0</v>
@@ -991,6 +1024,9 @@
         <v>0</v>
       </c>
       <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1050,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J16" t="n">
         <v>0</v>
@@ -1059,6 +1095,9 @@
         <v>0</v>
       </c>
       <c r="L16" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1094,7 +1133,7 @@
         <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J17" t="n">
         <v>0</v>
@@ -1103,6 +1142,9 @@
         <v>0</v>
       </c>
       <c r="L17" t="n">
+        <v>0</v>
+      </c>
+      <c r="M17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1138,7 +1180,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J18" t="n">
         <v>0</v>
@@ -1147,6 +1189,9 @@
         <v>0</v>
       </c>
       <c r="L18" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1182,7 +1227,7 @@
         <v>0</v>
       </c>
       <c r="I19" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J19" t="n">
         <v>0</v>
@@ -1191,6 +1236,9 @@
         <v>0</v>
       </c>
       <c r="L19" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1249,7 +1297,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J21" t="n">
         <v>0</v>
@@ -1258,6 +1306,9 @@
         <v>0</v>
       </c>
       <c r="L21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1293,7 +1344,7 @@
         <v>0</v>
       </c>
       <c r="I22" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J22" t="n">
         <v>0</v>
@@ -1302,6 +1353,9 @@
         <v>0</v>
       </c>
       <c r="L22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1337,7 +1391,7 @@
         <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J23" t="n">
         <v>0</v>
@@ -1346,6 +1400,9 @@
         <v>0</v>
       </c>
       <c r="L23" t="n">
+        <v>0</v>
+      </c>
+      <c r="M23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1381,7 +1438,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J24" t="n">
         <v>0</v>
@@ -1390,6 +1447,9 @@
         <v>0</v>
       </c>
       <c r="L24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1425,7 +1485,7 @@
         <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J25" t="n">
         <v>0</v>
@@ -1434,6 +1494,9 @@
         <v>0</v>
       </c>
       <c r="L25" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1469,7 +1532,7 @@
         <v>0</v>
       </c>
       <c r="I26" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J26" t="n">
         <v>0</v>
@@ -1478,6 +1541,9 @@
         <v>0</v>
       </c>
       <c r="L26" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1536,7 +1602,7 @@
         <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J28" t="n">
         <v>0</v>
@@ -1545,6 +1611,9 @@
         <v>0</v>
       </c>
       <c r="L28" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1580,7 +1649,7 @@
         <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J29" t="n">
         <v>0</v>
@@ -1589,6 +1658,9 @@
         <v>0</v>
       </c>
       <c r="L29" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1624,7 +1696,7 @@
         <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J30" t="n">
         <v>0</v>
@@ -1633,6 +1705,9 @@
         <v>0</v>
       </c>
       <c r="L30" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1668,7 +1743,7 @@
         <v>0</v>
       </c>
       <c r="I31" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J31" t="n">
         <v>0</v>
@@ -1677,6 +1752,9 @@
         <v>0</v>
       </c>
       <c r="L31" t="n">
+        <v>0</v>
+      </c>
+      <c r="M31" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1712,7 +1790,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J32" t="n">
         <v>0</v>
@@ -1721,6 +1799,9 @@
         <v>0</v>
       </c>
       <c r="L32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1756,7 +1837,7 @@
         <v>0</v>
       </c>
       <c r="I33" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J33" t="n">
         <v>0</v>
@@ -1765,6 +1846,9 @@
         <v>0</v>
       </c>
       <c r="L33" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1800,7 +1884,7 @@
         <v>0</v>
       </c>
       <c r="I34" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J34" t="n">
         <v>0</v>
@@ -1809,6 +1893,9 @@
         <v>0</v>
       </c>
       <c r="L34" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1868,7 +1955,7 @@
         <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J36" t="n">
         <v>0</v>
@@ -1877,6 +1964,9 @@
         <v>0</v>
       </c>
       <c r="L36" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1912,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J37" t="n">
         <v>0</v>
@@ -1921,6 +2011,9 @@
         <v>0</v>
       </c>
       <c r="L37" t="n">
+        <v>0</v>
+      </c>
+      <c r="M37" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1979,7 +2072,7 @@
         <v>0</v>
       </c>
       <c r="I39" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J39" t="n">
         <v>0</v>
@@ -1988,6 +2081,9 @@
         <v>0</v>
       </c>
       <c r="L39" t="n">
+        <v>0</v>
+      </c>
+      <c r="M39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2023,7 +2119,7 @@
         <v>0</v>
       </c>
       <c r="I40" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J40" t="n">
         <v>0</v>
@@ -2032,6 +2128,9 @@
         <v>0</v>
       </c>
       <c r="L40" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2067,7 +2166,7 @@
         <v>0</v>
       </c>
       <c r="I41" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J41" t="n">
         <v>0</v>
@@ -2076,6 +2175,9 @@
         <v>0</v>
       </c>
       <c r="L41" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2111,7 +2213,7 @@
         <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J42" t="n">
         <v>0</v>
@@ -2120,6 +2222,9 @@
         <v>0</v>
       </c>
       <c r="L42" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2155,7 +2260,7 @@
         <v>0</v>
       </c>
       <c r="I43" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J43" t="n">
         <v>0</v>
@@ -2164,6 +2269,9 @@
         <v>0</v>
       </c>
       <c r="L43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M43" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2199,7 +2307,7 @@
         <v>0</v>
       </c>
       <c r="I44" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J44" t="n">
         <v>0</v>
@@ -2208,6 +2316,9 @@
         <v>0</v>
       </c>
       <c r="L44" t="n">
+        <v>0</v>
+      </c>
+      <c r="M44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2243,7 +2354,7 @@
         <v>0</v>
       </c>
       <c r="I45" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J45" t="n">
         <v>0</v>
@@ -2252,6 +2363,9 @@
         <v>0</v>
       </c>
       <c r="L45" t="n">
+        <v>0</v>
+      </c>
+      <c r="M45" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2287,7 +2401,7 @@
         <v>0</v>
       </c>
       <c r="I46" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J46" t="n">
         <v>0</v>
@@ -2296,6 +2410,9 @@
         <v>0</v>
       </c>
       <c r="L46" t="n">
+        <v>0</v>
+      </c>
+      <c r="M46" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2354,7 +2471,7 @@
         <v>0</v>
       </c>
       <c r="I48" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J48" t="n">
         <v>0</v>
@@ -2363,6 +2480,9 @@
         <v>0</v>
       </c>
       <c r="L48" t="n">
+        <v>0</v>
+      </c>
+      <c r="M48" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2398,7 +2518,7 @@
         <v>0</v>
       </c>
       <c r="I49" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J49" t="n">
         <v>0</v>
@@ -2407,6 +2527,9 @@
         <v>0</v>
       </c>
       <c r="L49" t="n">
+        <v>0</v>
+      </c>
+      <c r="M49" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2442,7 +2565,7 @@
         <v>0</v>
       </c>
       <c r="I50" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J50" t="n">
         <v>0</v>
@@ -2451,6 +2574,9 @@
         <v>0</v>
       </c>
       <c r="L50" t="n">
+        <v>0</v>
+      </c>
+      <c r="M50" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2486,7 +2612,7 @@
         <v>0</v>
       </c>
       <c r="I51" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J51" t="n">
         <v>0</v>
@@ -2495,6 +2621,9 @@
         <v>0</v>
       </c>
       <c r="L51" t="n">
+        <v>0</v>
+      </c>
+      <c r="M51" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2530,7 +2659,7 @@
         <v>0</v>
       </c>
       <c r="I52" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J52" t="n">
         <v>0</v>
@@ -2539,6 +2668,9 @@
         <v>0</v>
       </c>
       <c r="L52" t="n">
+        <v>0</v>
+      </c>
+      <c r="M52" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2574,7 +2706,7 @@
         <v>0</v>
       </c>
       <c r="I53" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J53" t="n">
         <v>0</v>
@@ -2583,6 +2715,9 @@
         <v>0</v>
       </c>
       <c r="L53" t="n">
+        <v>0</v>
+      </c>
+      <c r="M53" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2618,7 +2753,7 @@
         <v>0</v>
       </c>
       <c r="I54" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J54" t="n">
         <v>0</v>
@@ -2627,6 +2762,9 @@
         <v>0</v>
       </c>
       <c r="L54" t="n">
+        <v>0</v>
+      </c>
+      <c r="M54" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2662,7 +2800,7 @@
         <v>0</v>
       </c>
       <c r="I55" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J55" t="n">
         <v>0</v>
@@ -2671,6 +2809,9 @@
         <v>0</v>
       </c>
       <c r="L55" t="n">
+        <v>0</v>
+      </c>
+      <c r="M55" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2706,7 +2847,7 @@
         <v>0</v>
       </c>
       <c r="I56" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J56" t="n">
         <v>0</v>
@@ -2715,6 +2856,9 @@
         <v>0</v>
       </c>
       <c r="L56" t="n">
+        <v>0</v>
+      </c>
+      <c r="M56" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2773,7 +2917,7 @@
         <v>0</v>
       </c>
       <c r="I58" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J58" t="n">
         <v>0</v>
@@ -2782,6 +2926,9 @@
         <v>0</v>
       </c>
       <c r="L58" t="n">
+        <v>0</v>
+      </c>
+      <c r="M58" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2817,7 +2964,7 @@
         <v>0</v>
       </c>
       <c r="I59" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J59" t="n">
         <v>0</v>
@@ -2826,6 +2973,9 @@
         <v>0</v>
       </c>
       <c r="L59" t="n">
+        <v>0</v>
+      </c>
+      <c r="M59" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2861,7 +3011,7 @@
         <v>0</v>
       </c>
       <c r="I60" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J60" t="n">
         <v>0</v>
@@ -2870,6 +3020,9 @@
         <v>0</v>
       </c>
       <c r="L60" t="n">
+        <v>0</v>
+      </c>
+      <c r="M60" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2905,7 +3058,7 @@
         <v>0</v>
       </c>
       <c r="I61" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J61" t="n">
         <v>0</v>
@@ -2914,6 +3067,9 @@
         <v>0</v>
       </c>
       <c r="L61" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2949,7 +3105,7 @@
         <v>0</v>
       </c>
       <c r="I62" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J62" t="n">
         <v>0</v>
@@ -2958,6 +3114,9 @@
         <v>0</v>
       </c>
       <c r="L62" t="n">
+        <v>0</v>
+      </c>
+      <c r="M62" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2993,7 +3152,7 @@
         <v>0</v>
       </c>
       <c r="I63" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J63" t="n">
         <v>0</v>
@@ -3002,6 +3161,9 @@
         <v>0</v>
       </c>
       <c r="L63" t="n">
+        <v>0</v>
+      </c>
+      <c r="M63" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3037,7 +3199,7 @@
         <v>0</v>
       </c>
       <c r="I64" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J64" t="n">
         <v>0</v>
@@ -3046,6 +3208,9 @@
         <v>0</v>
       </c>
       <c r="L64" t="n">
+        <v>0</v>
+      </c>
+      <c r="M64" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3081,7 +3246,7 @@
         <v>0</v>
       </c>
       <c r="I65" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J65" t="n">
         <v>0</v>
@@ -3090,6 +3255,9 @@
         <v>0</v>
       </c>
       <c r="L65" t="n">
+        <v>0</v>
+      </c>
+      <c r="M65" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3125,7 +3293,7 @@
         <v>0</v>
       </c>
       <c r="I66" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J66" t="n">
         <v>0</v>
@@ -3134,6 +3302,9 @@
         <v>0</v>
       </c>
       <c r="L66" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3192,7 +3363,7 @@
         <v>0</v>
       </c>
       <c r="I68" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J68" t="n">
         <v>0</v>
@@ -3201,6 +3372,9 @@
         <v>0</v>
       </c>
       <c r="L68" t="n">
+        <v>0</v>
+      </c>
+      <c r="M68" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3260,7 +3434,7 @@
         <v>0</v>
       </c>
       <c r="I70" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J70" t="n">
         <v>0</v>
@@ -3269,6 +3443,9 @@
         <v>0</v>
       </c>
       <c r="L70" t="n">
+        <v>0</v>
+      </c>
+      <c r="M70" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3304,7 +3481,7 @@
         <v>0</v>
       </c>
       <c r="I71" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J71" t="n">
         <v>0</v>
@@ -3313,6 +3490,9 @@
         <v>0</v>
       </c>
       <c r="L71" t="n">
+        <v>0</v>
+      </c>
+      <c r="M71" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3348,7 +3528,7 @@
         <v>0</v>
       </c>
       <c r="I72" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J72" t="n">
         <v>0</v>
@@ -3357,6 +3537,9 @@
         <v>0</v>
       </c>
       <c r="L72" t="n">
+        <v>0</v>
+      </c>
+      <c r="M72" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3392,7 +3575,7 @@
         <v>0</v>
       </c>
       <c r="I73" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J73" t="n">
         <v>0</v>
@@ -3401,6 +3584,9 @@
         <v>0</v>
       </c>
       <c r="L73" t="n">
+        <v>0</v>
+      </c>
+      <c r="M73" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3460,7 +3646,7 @@
         <v>0</v>
       </c>
       <c r="I75" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J75" t="n">
         <v>0</v>
@@ -3469,6 +3655,9 @@
         <v>0</v>
       </c>
       <c r="L75" t="n">
+        <v>0</v>
+      </c>
+      <c r="M75" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3504,7 +3693,7 @@
         <v>0</v>
       </c>
       <c r="I76" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J76" t="n">
         <v>0</v>
@@ -3513,6 +3702,9 @@
         <v>0</v>
       </c>
       <c r="L76" t="n">
+        <v>0</v>
+      </c>
+      <c r="M76" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3548,7 +3740,7 @@
         <v>0</v>
       </c>
       <c r="I77" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J77" t="n">
         <v>0</v>
@@ -3557,6 +3749,9 @@
         <v>0</v>
       </c>
       <c r="L77" t="n">
+        <v>0</v>
+      </c>
+      <c r="M77" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3615,7 +3810,7 @@
         <v>0</v>
       </c>
       <c r="I79" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J79" t="n">
         <v>0</v>
@@ -3624,6 +3819,9 @@
         <v>0</v>
       </c>
       <c r="L79" t="n">
+        <v>0</v>
+      </c>
+      <c r="M79" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3659,7 +3857,7 @@
         <v>0</v>
       </c>
       <c r="I80" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J80" t="n">
         <v>0</v>
@@ -3668,6 +3866,9 @@
         <v>0</v>
       </c>
       <c r="L80" t="n">
+        <v>0</v>
+      </c>
+      <c r="M80" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3703,7 +3904,7 @@
         <v>0</v>
       </c>
       <c r="I81" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J81" t="n">
         <v>0</v>
@@ -3712,6 +3913,9 @@
         <v>0</v>
       </c>
       <c r="L81" t="n">
+        <v>0</v>
+      </c>
+      <c r="M81" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3747,7 +3951,7 @@
         <v>0</v>
       </c>
       <c r="I82" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J82" t="n">
         <v>0</v>
@@ -3756,6 +3960,9 @@
         <v>0</v>
       </c>
       <c r="L82" t="n">
+        <v>0</v>
+      </c>
+      <c r="M82" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3791,7 +3998,7 @@
         <v>0</v>
       </c>
       <c r="I83" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J83" t="n">
         <v>0</v>
@@ -3800,6 +4007,9 @@
         <v>0</v>
       </c>
       <c r="L83" t="n">
+        <v>0</v>
+      </c>
+      <c r="M83" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3835,7 +4045,7 @@
         <v>0</v>
       </c>
       <c r="I84" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J84" t="n">
         <v>0</v>
@@ -3844,6 +4054,9 @@
         <v>0</v>
       </c>
       <c r="L84" t="n">
+        <v>0</v>
+      </c>
+      <c r="M84" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3879,7 +4092,7 @@
         <v>0</v>
       </c>
       <c r="I85" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J85" t="n">
         <v>0</v>
@@ -3888,6 +4101,9 @@
         <v>0</v>
       </c>
       <c r="L85" t="n">
+        <v>0</v>
+      </c>
+      <c r="M85" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3923,7 +4139,7 @@
         <v>0</v>
       </c>
       <c r="I86" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J86" t="n">
         <v>0</v>
@@ -3932,6 +4148,9 @@
         <v>0</v>
       </c>
       <c r="L86" t="n">
+        <v>0</v>
+      </c>
+      <c r="M86" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3990,7 +4209,7 @@
         <v>0</v>
       </c>
       <c r="I88" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J88" t="n">
         <v>0</v>
@@ -3999,6 +4218,9 @@
         <v>0</v>
       </c>
       <c r="L88" t="n">
+        <v>0</v>
+      </c>
+      <c r="M88" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4034,7 +4256,7 @@
         <v>0</v>
       </c>
       <c r="I89" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J89" t="n">
         <v>0</v>
@@ -4043,6 +4265,9 @@
         <v>0</v>
       </c>
       <c r="L89" t="n">
+        <v>0</v>
+      </c>
+      <c r="M89" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4078,7 +4303,7 @@
         <v>0</v>
       </c>
       <c r="I90" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J90" t="n">
         <v>0</v>
@@ -4087,6 +4312,9 @@
         <v>0</v>
       </c>
       <c r="L90" t="n">
+        <v>0</v>
+      </c>
+      <c r="M90" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4146,7 +4374,7 @@
         <v>0</v>
       </c>
       <c r="I92" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J92" t="n">
         <v>0</v>
@@ -4155,6 +4383,9 @@
         <v>0</v>
       </c>
       <c r="L92" t="n">
+        <v>0</v>
+      </c>
+      <c r="M92" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4213,7 +4444,7 @@
         <v>0</v>
       </c>
       <c r="I94" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J94" t="n">
         <v>0</v>
@@ -4222,6 +4453,9 @@
         <v>0</v>
       </c>
       <c r="L94" t="n">
+        <v>0</v>
+      </c>
+      <c r="M94" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4257,7 +4491,7 @@
         <v>0</v>
       </c>
       <c r="I95" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J95" t="n">
         <v>0</v>
@@ -4266,6 +4500,9 @@
         <v>0</v>
       </c>
       <c r="L95" t="n">
+        <v>0</v>
+      </c>
+      <c r="M95" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4301,7 +4538,7 @@
         <v>0</v>
       </c>
       <c r="I96" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J96" t="n">
         <v>0</v>
@@ -4310,6 +4547,9 @@
         <v>0</v>
       </c>
       <c r="L96" t="n">
+        <v>0</v>
+      </c>
+      <c r="M96" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4345,7 +4585,7 @@
         <v>0</v>
       </c>
       <c r="I97" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J97" t="n">
         <v>0</v>
@@ -4354,6 +4594,9 @@
         <v>0</v>
       </c>
       <c r="L97" t="n">
+        <v>0</v>
+      </c>
+      <c r="M97" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4389,7 +4632,7 @@
         <v>0</v>
       </c>
       <c r="I98" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J98" t="n">
         <v>0</v>
@@ -4398,6 +4641,9 @@
         <v>0</v>
       </c>
       <c r="L98" t="n">
+        <v>0</v>
+      </c>
+      <c r="M98" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4433,7 +4679,7 @@
         <v>0</v>
       </c>
       <c r="I99" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J99" t="n">
         <v>0</v>
@@ -4442,6 +4688,9 @@
         <v>0</v>
       </c>
       <c r="L99" t="n">
+        <v>0</v>
+      </c>
+      <c r="M99" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4477,7 +4726,7 @@
         <v>0</v>
       </c>
       <c r="I100" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J100" t="n">
         <v>0</v>
@@ -4486,6 +4735,9 @@
         <v>0</v>
       </c>
       <c r="L100" t="n">
+        <v>0</v>
+      </c>
+      <c r="M100" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4521,7 +4773,7 @@
         <v>0</v>
       </c>
       <c r="I101" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J101" t="n">
         <v>0</v>
@@ -4530,6 +4782,9 @@
         <v>0</v>
       </c>
       <c r="L101" t="n">
+        <v>0</v>
+      </c>
+      <c r="M101" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4589,7 +4844,7 @@
         <v>0</v>
       </c>
       <c r="I103" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J103" t="n">
         <v>0</v>
@@ -4598,6 +4853,9 @@
         <v>0</v>
       </c>
       <c r="L103" t="n">
+        <v>0</v>
+      </c>
+      <c r="M103" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4633,7 +4891,7 @@
         <v>0</v>
       </c>
       <c r="I104" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J104" t="n">
         <v>0</v>
@@ -4642,6 +4900,9 @@
         <v>0</v>
       </c>
       <c r="L104" t="n">
+        <v>0</v>
+      </c>
+      <c r="M104" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4677,7 +4938,7 @@
         <v>0</v>
       </c>
       <c r="I105" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J105" t="n">
         <v>0</v>
@@ -4686,6 +4947,9 @@
         <v>0</v>
       </c>
       <c r="L105" t="n">
+        <v>0</v>
+      </c>
+      <c r="M105" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4744,7 +5008,7 @@
         <v>0</v>
       </c>
       <c r="I107" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J107" t="n">
         <v>0</v>
@@ -4753,6 +5017,9 @@
         <v>0</v>
       </c>
       <c r="L107" t="n">
+        <v>0</v>
+      </c>
+      <c r="M107" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4788,7 +5055,7 @@
         <v>0</v>
       </c>
       <c r="I108" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J108" t="n">
         <v>0</v>
@@ -4797,6 +5064,9 @@
         <v>0</v>
       </c>
       <c r="L108" t="n">
+        <v>0</v>
+      </c>
+      <c r="M108" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4832,7 +5102,7 @@
         <v>-1</v>
       </c>
       <c r="I109" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J109" t="n">
         <v>0</v>
@@ -4842,6 +5112,9 @@
       </c>
       <c r="L109" t="n">
         <v>0</v>
+      </c>
+      <c r="M109" t="n">
+        <v>-2</v>
       </c>
     </row>
     <row r="110">
@@ -4876,7 +5149,7 @@
         <v>0</v>
       </c>
       <c r="I110" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J110" t="n">
         <v>0</v>
@@ -4886,6 +5159,9 @@
       </c>
       <c r="L110" t="n">
         <v>0</v>
+      </c>
+      <c r="M110" t="n">
+        <v>-2</v>
       </c>
     </row>
     <row r="111">
@@ -4920,7 +5196,7 @@
         <v>1</v>
       </c>
       <c r="I111" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J111" t="n">
         <v>0</v>
@@ -4929,6 +5205,9 @@
         <v>0</v>
       </c>
       <c r="L111" t="n">
+        <v>0</v>
+      </c>
+      <c r="M111" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4964,7 +5243,7 @@
         <v>0</v>
       </c>
       <c r="I112" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J112" t="n">
         <v>0</v>
@@ -4973,6 +5252,9 @@
         <v>0</v>
       </c>
       <c r="L112" t="n">
+        <v>0</v>
+      </c>
+      <c r="M112" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5008,7 +5290,7 @@
         <v>0</v>
       </c>
       <c r="I113" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J113" t="n">
         <v>0</v>
@@ -5017,6 +5299,9 @@
         <v>0</v>
       </c>
       <c r="L113" t="n">
+        <v>0</v>
+      </c>
+      <c r="M113" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5052,7 +5337,7 @@
         <v>0</v>
       </c>
       <c r="I114" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J114" t="n">
         <v>0</v>
@@ -5061,6 +5346,9 @@
         <v>0</v>
       </c>
       <c r="L114" t="n">
+        <v>0</v>
+      </c>
+      <c r="M114" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5119,7 +5407,7 @@
         <v>0</v>
       </c>
       <c r="I116" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J116" t="n">
         <v>0</v>
@@ -5128,6 +5416,9 @@
         <v>0</v>
       </c>
       <c r="L116" t="n">
+        <v>0</v>
+      </c>
+      <c r="M116" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5163,7 +5454,7 @@
         <v>0</v>
       </c>
       <c r="I117" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J117" t="n">
         <v>0</v>
@@ -5172,6 +5463,9 @@
         <v>0</v>
       </c>
       <c r="L117" t="n">
+        <v>0</v>
+      </c>
+      <c r="M117" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5207,7 +5501,7 @@
         <v>0</v>
       </c>
       <c r="I118" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J118" t="n">
         <v>0</v>
@@ -5216,6 +5510,9 @@
         <v>0</v>
       </c>
       <c r="L118" t="n">
+        <v>0</v>
+      </c>
+      <c r="M118" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5251,7 +5548,7 @@
         <v>0</v>
       </c>
       <c r="I119" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J119" t="n">
         <v>0</v>
@@ -5260,6 +5557,9 @@
         <v>0</v>
       </c>
       <c r="L119" t="n">
+        <v>0</v>
+      </c>
+      <c r="M119" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5295,7 +5595,7 @@
         <v>0</v>
       </c>
       <c r="I120" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J120" t="n">
         <v>0</v>
@@ -5304,6 +5604,9 @@
         <v>0</v>
       </c>
       <c r="L120" t="n">
+        <v>0</v>
+      </c>
+      <c r="M120" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5339,7 +5642,7 @@
         <v>0</v>
       </c>
       <c r="I121" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J121" t="n">
         <v>0</v>
@@ -5348,6 +5651,9 @@
         <v>0</v>
       </c>
       <c r="L121" t="n">
+        <v>0</v>
+      </c>
+      <c r="M121" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5383,7 +5689,7 @@
         <v>0</v>
       </c>
       <c r="I122" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J122" t="n">
         <v>0</v>
@@ -5392,6 +5698,9 @@
         <v>0</v>
       </c>
       <c r="L122" t="n">
+        <v>0</v>
+      </c>
+      <c r="M122" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5427,7 +5736,7 @@
         <v>0</v>
       </c>
       <c r="I123" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J123" t="n">
         <v>0</v>
@@ -5436,6 +5745,9 @@
         <v>0</v>
       </c>
       <c r="L123" t="n">
+        <v>0</v>
+      </c>
+      <c r="M123" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5471,7 +5783,7 @@
         <v>0</v>
       </c>
       <c r="I124" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J124" t="n">
         <v>0</v>
@@ -5480,6 +5792,9 @@
         <v>0</v>
       </c>
       <c r="L124" t="n">
+        <v>0</v>
+      </c>
+      <c r="M124" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5538,7 +5853,7 @@
         <v>0</v>
       </c>
       <c r="I126" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J126" t="n">
         <v>0</v>
@@ -5547,6 +5862,9 @@
         <v>0</v>
       </c>
       <c r="L126" t="n">
+        <v>0</v>
+      </c>
+      <c r="M126" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5582,7 +5900,7 @@
         <v>0</v>
       </c>
       <c r="I127" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J127" t="n">
         <v>0</v>
@@ -5591,6 +5909,9 @@
         <v>0</v>
       </c>
       <c r="L127" t="n">
+        <v>0</v>
+      </c>
+      <c r="M127" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5626,7 +5947,7 @@
         <v>0</v>
       </c>
       <c r="I128" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J128" t="n">
         <v>0</v>
@@ -5635,6 +5956,9 @@
         <v>0</v>
       </c>
       <c r="L128" t="n">
+        <v>0</v>
+      </c>
+      <c r="M128" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5670,7 +5994,7 @@
         <v>0</v>
       </c>
       <c r="I129" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J129" t="n">
         <v>0</v>
@@ -5679,6 +6003,9 @@
         <v>0</v>
       </c>
       <c r="L129" t="n">
+        <v>0</v>
+      </c>
+      <c r="M129" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5714,7 +6041,7 @@
         <v>0</v>
       </c>
       <c r="I130" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J130" t="n">
         <v>0</v>
@@ -5723,6 +6050,9 @@
         <v>0</v>
       </c>
       <c r="L130" t="n">
+        <v>0</v>
+      </c>
+      <c r="M130" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5758,7 +6088,7 @@
         <v>0</v>
       </c>
       <c r="I131" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J131" t="n">
         <v>0</v>
@@ -5767,6 +6097,9 @@
         <v>0</v>
       </c>
       <c r="L131" t="n">
+        <v>0</v>
+      </c>
+      <c r="M131" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5802,7 +6135,7 @@
         <v>0</v>
       </c>
       <c r="I132" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J132" t="n">
         <v>0</v>
@@ -5811,6 +6144,9 @@
         <v>0</v>
       </c>
       <c r="L132" t="n">
+        <v>0</v>
+      </c>
+      <c r="M132" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5846,7 +6182,7 @@
         <v>0</v>
       </c>
       <c r="I133" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J133" t="n">
         <v>0</v>
@@ -5855,6 +6191,9 @@
         <v>0</v>
       </c>
       <c r="L133" t="n">
+        <v>0</v>
+      </c>
+      <c r="M133" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5890,7 +6229,7 @@
         <v>0</v>
       </c>
       <c r="I134" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J134" t="n">
         <v>0</v>
@@ -5899,6 +6238,9 @@
         <v>0</v>
       </c>
       <c r="L134" t="n">
+        <v>0</v>
+      </c>
+      <c r="M134" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5957,7 +6299,7 @@
         <v>0</v>
       </c>
       <c r="I136" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J136" t="n">
         <v>0</v>
@@ -5966,6 +6308,9 @@
         <v>0</v>
       </c>
       <c r="L136" t="n">
+        <v>0</v>
+      </c>
+      <c r="M136" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6001,7 +6346,7 @@
         <v>0</v>
       </c>
       <c r="I137" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J137" t="n">
         <v>0</v>
@@ -6010,6 +6355,9 @@
         <v>0</v>
       </c>
       <c r="L137" t="n">
+        <v>0</v>
+      </c>
+      <c r="M137" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6045,7 +6393,7 @@
         <v>0</v>
       </c>
       <c r="I138" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J138" t="n">
         <v>0</v>
@@ -6054,6 +6402,9 @@
         <v>0</v>
       </c>
       <c r="L138" t="n">
+        <v>0</v>
+      </c>
+      <c r="M138" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6089,7 +6440,7 @@
         <v>0</v>
       </c>
       <c r="I139" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J139" t="n">
         <v>0</v>
@@ -6098,6 +6449,9 @@
         <v>0</v>
       </c>
       <c r="L139" t="n">
+        <v>0</v>
+      </c>
+      <c r="M139" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6133,7 +6487,7 @@
         <v>0</v>
       </c>
       <c r="I140" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J140" t="n">
         <v>0</v>
@@ -6142,6 +6496,9 @@
         <v>0</v>
       </c>
       <c r="L140" t="n">
+        <v>0</v>
+      </c>
+      <c r="M140" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6177,7 +6534,7 @@
         <v>0</v>
       </c>
       <c r="I141" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J141" t="n">
         <v>0</v>
@@ -6186,6 +6543,9 @@
         <v>0</v>
       </c>
       <c r="L141" t="n">
+        <v>0</v>
+      </c>
+      <c r="M141" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6221,7 +6581,7 @@
         <v>0</v>
       </c>
       <c r="I142" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J142" t="n">
         <v>0</v>
@@ -6230,6 +6590,9 @@
         <v>0</v>
       </c>
       <c r="L142" t="n">
+        <v>0</v>
+      </c>
+      <c r="M142" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6265,7 +6628,7 @@
         <v>0</v>
       </c>
       <c r="I143" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J143" t="n">
         <v>0</v>
@@ -6274,6 +6637,9 @@
         <v>0</v>
       </c>
       <c r="L143" t="n">
+        <v>0</v>
+      </c>
+      <c r="M143" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6309,7 +6675,7 @@
         <v>0</v>
       </c>
       <c r="I144" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J144" t="n">
         <v>0</v>
@@ -6318,6 +6684,9 @@
         <v>0</v>
       </c>
       <c r="L144" t="n">
+        <v>0</v>
+      </c>
+      <c r="M144" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6376,7 +6745,7 @@
         <v>0</v>
       </c>
       <c r="I146" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J146" t="n">
         <v>0</v>
@@ -6385,6 +6754,9 @@
         <v>0</v>
       </c>
       <c r="L146" t="n">
+        <v>0</v>
+      </c>
+      <c r="M146" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6420,7 +6792,7 @@
         <v>0</v>
       </c>
       <c r="I147" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J147" t="n">
         <v>0</v>
@@ -6429,6 +6801,9 @@
         <v>0</v>
       </c>
       <c r="L147" t="n">
+        <v>0</v>
+      </c>
+      <c r="M147" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6464,7 +6839,7 @@
         <v>0</v>
       </c>
       <c r="I148" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J148" t="n">
         <v>0</v>
@@ -6473,6 +6848,9 @@
         <v>0</v>
       </c>
       <c r="L148" t="n">
+        <v>0</v>
+      </c>
+      <c r="M148" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6508,7 +6886,7 @@
         <v>0</v>
       </c>
       <c r="I149" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J149" t="n">
         <v>0</v>
@@ -6517,6 +6895,9 @@
         <v>0</v>
       </c>
       <c r="L149" t="n">
+        <v>0</v>
+      </c>
+      <c r="M149" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6552,7 +6933,7 @@
         <v>0</v>
       </c>
       <c r="I150" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J150" t="n">
         <v>0</v>
@@ -6561,6 +6942,9 @@
         <v>0</v>
       </c>
       <c r="L150" t="n">
+        <v>0</v>
+      </c>
+      <c r="M150" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6596,7 +6980,7 @@
         <v>0</v>
       </c>
       <c r="I151" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J151" t="n">
         <v>0</v>
@@ -6605,6 +6989,9 @@
         <v>0</v>
       </c>
       <c r="L151" t="n">
+        <v>0</v>
+      </c>
+      <c r="M151" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6640,7 +7027,7 @@
         <v>0</v>
       </c>
       <c r="I152" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J152" t="n">
         <v>0</v>
@@ -6649,6 +7036,9 @@
         <v>0</v>
       </c>
       <c r="L152" t="n">
+        <v>0</v>
+      </c>
+      <c r="M152" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6684,7 +7074,7 @@
         <v>0</v>
       </c>
       <c r="I153" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J153" t="n">
         <v>0</v>
@@ -6693,6 +7083,9 @@
         <v>0</v>
       </c>
       <c r="L153" t="n">
+        <v>0</v>
+      </c>
+      <c r="M153" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6728,7 +7121,7 @@
         <v>0</v>
       </c>
       <c r="I154" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J154" t="n">
         <v>0</v>
@@ -6737,6 +7130,9 @@
         <v>0</v>
       </c>
       <c r="L154" t="n">
+        <v>0</v>
+      </c>
+      <c r="M154" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6795,7 +7191,7 @@
         <v>0</v>
       </c>
       <c r="I156" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J156" t="n">
         <v>0</v>
@@ -6804,6 +7200,9 @@
         <v>0</v>
       </c>
       <c r="L156" t="n">
+        <v>0</v>
+      </c>
+      <c r="M156" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6839,7 +7238,7 @@
         <v>0</v>
       </c>
       <c r="I157" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J157" t="n">
         <v>0</v>
@@ -6848,6 +7247,9 @@
         <v>0</v>
       </c>
       <c r="L157" t="n">
+        <v>0</v>
+      </c>
+      <c r="M157" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6883,7 +7285,7 @@
         <v>0</v>
       </c>
       <c r="I158" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J158" t="n">
         <v>0</v>
@@ -6892,6 +7294,9 @@
         <v>0</v>
       </c>
       <c r="L158" t="n">
+        <v>0</v>
+      </c>
+      <c r="M158" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6927,7 +7332,7 @@
         <v>0</v>
       </c>
       <c r="I159" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J159" t="n">
         <v>0</v>
@@ -6936,6 +7341,9 @@
         <v>0</v>
       </c>
       <c r="L159" t="n">
+        <v>0</v>
+      </c>
+      <c r="M159" t="n">
         <v>0</v>
       </c>
     </row>
@@ -6971,7 +7379,7 @@
         <v>0</v>
       </c>
       <c r="I160" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J160" t="n">
         <v>0</v>
@@ -6980,6 +7388,9 @@
         <v>0</v>
       </c>
       <c r="L160" t="n">
+        <v>0</v>
+      </c>
+      <c r="M160" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7015,7 +7426,7 @@
         <v>0</v>
       </c>
       <c r="I161" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J161" t="n">
         <v>0</v>
@@ -7024,6 +7435,9 @@
         <v>0</v>
       </c>
       <c r="L161" t="n">
+        <v>0</v>
+      </c>
+      <c r="M161" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7059,7 +7473,7 @@
         <v>0</v>
       </c>
       <c r="I162" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J162" t="n">
         <v>0</v>
@@ -7068,6 +7482,9 @@
         <v>0</v>
       </c>
       <c r="L162" t="n">
+        <v>0</v>
+      </c>
+      <c r="M162" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7103,7 +7520,7 @@
         <v>0</v>
       </c>
       <c r="I163" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J163" t="n">
         <v>0</v>
@@ -7112,6 +7529,9 @@
         <v>0</v>
       </c>
       <c r="L163" t="n">
+        <v>0</v>
+      </c>
+      <c r="M163" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7147,7 +7567,7 @@
         <v>0</v>
       </c>
       <c r="I164" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J164" t="n">
         <v>0</v>
@@ -7156,6 +7576,9 @@
         <v>0</v>
       </c>
       <c r="L164" t="n">
+        <v>0</v>
+      </c>
+      <c r="M164" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7214,7 +7637,7 @@
         <v>0</v>
       </c>
       <c r="I166" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J166" t="n">
         <v>0</v>
@@ -7223,6 +7646,9 @@
         <v>0</v>
       </c>
       <c r="L166" t="n">
+        <v>0</v>
+      </c>
+      <c r="M166" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7258,7 +7684,7 @@
         <v>0</v>
       </c>
       <c r="I167" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J167" t="n">
         <v>0</v>
@@ -7267,6 +7693,9 @@
         <v>0</v>
       </c>
       <c r="L167" t="n">
+        <v>0</v>
+      </c>
+      <c r="M167" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7302,7 +7731,7 @@
         <v>0</v>
       </c>
       <c r="I168" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J168" t="n">
         <v>0</v>
@@ -7311,6 +7740,9 @@
         <v>0</v>
       </c>
       <c r="L168" t="n">
+        <v>0</v>
+      </c>
+      <c r="M168" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7346,7 +7778,7 @@
         <v>0</v>
       </c>
       <c r="I169" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J169" t="n">
         <v>0</v>
@@ -7355,6 +7787,9 @@
         <v>0</v>
       </c>
       <c r="L169" t="n">
+        <v>0</v>
+      </c>
+      <c r="M169" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7390,7 +7825,7 @@
         <v>0</v>
       </c>
       <c r="I170" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J170" t="n">
         <v>0</v>
@@ -7399,6 +7834,9 @@
         <v>0</v>
       </c>
       <c r="L170" t="n">
+        <v>0</v>
+      </c>
+      <c r="M170" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7434,7 +7872,7 @@
         <v>0</v>
       </c>
       <c r="I171" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J171" t="n">
         <v>0</v>
@@ -7443,6 +7881,9 @@
         <v>0</v>
       </c>
       <c r="L171" t="n">
+        <v>0</v>
+      </c>
+      <c r="M171" t="n">
         <v>0</v>
       </c>
     </row>
@@ -7478,7 +7919,7 @@
         <v>0</v>
       </c>
       <c r="I172" t="n">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="J172" t="n">
         <v>0</v>
@@ -7487,6 +7928,9 @@
         <v>0</v>
       </c>
       <c r="L172" t="n">
+        <v>0</v>
+      </c>
+      <c r="M172" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated trackModel and Added connection signals
</commit_message>
<xml_diff>
--- a/TrackModel/src/database.xlsx
+++ b/TrackModel/src/database.xlsx
@@ -886,7 +886,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12">
@@ -1262,7 +1262,7 @@
         </is>
       </c>
       <c r="F20" t="n">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21">
@@ -1567,7 +1567,7 @@
         </is>
       </c>
       <c r="F27" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28">
@@ -2037,7 +2037,7 @@
         </is>
       </c>
       <c r="F38" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39">
@@ -2436,7 +2436,7 @@
         </is>
       </c>
       <c r="F47" t="n">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48">
@@ -2882,7 +2882,7 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="58">
@@ -3328,7 +3328,7 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="68">
@@ -3775,7 +3775,7 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="79">
@@ -4174,7 +4174,7 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="88">
@@ -4409,7 +4409,7 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="94">
@@ -4973,7 +4973,7 @@
         </is>
       </c>
       <c r="F106" t="n">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="107">
@@ -5372,7 +5372,7 @@
         </is>
       </c>
       <c r="F115" t="n">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="116">
@@ -5818,7 +5818,7 @@
         </is>
       </c>
       <c r="F125" t="n">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="126">
@@ -6264,7 +6264,7 @@
         </is>
       </c>
       <c r="F135" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="136">
@@ -6710,7 +6710,7 @@
         </is>
       </c>
       <c r="F145" t="n">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="146">
@@ -7602,7 +7602,7 @@
         </is>
       </c>
       <c r="F165" t="n">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="166">

</xml_diff>